<commit_message>
se cambio el nombre del Tag a crear pedido
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>TC1</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>C200061474</t>
+  </si>
+  <si>
+    <t>C200061488</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +206,11 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -267,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -300,7 +308,8 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -708,7 +717,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
se cambio la  configuracion de maven
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>TC1</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>C200061488</t>
+  </si>
+  <si>
+    <t>C200061502</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +209,11 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -275,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -309,7 +317,8 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -717,7 +726,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
se cambio la  configuracion de maven2
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>TC1</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>C200061502</t>
+  </si>
+  <si>
+    <t>C200061506</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +212,11 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -283,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -318,7 +326,8 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -726,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>